<commit_message>
generated Gerbers, updated BoM
</commit_message>
<xml_diff>
--- a/New PCB, no jumpers/Bill of Materials.xlsx
+++ b/New PCB, no jumpers/Bill of Materials.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kpezeshki\Desktop\MuddPIV5\New PCB, no jumpers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kpezeshki\Desktop\MuddPiV5\New PCB, no jumpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="uMudd Mark V" sheetId="1" r:id="rId1"/>
@@ -410,18 +410,6 @@
     <t>SAM download connector</t>
   </si>
   <si>
-    <t>Harwin</t>
-  </si>
-  <si>
-    <t>M52-040023W0545</t>
-  </si>
-  <si>
-    <t>855-M52-040023W0545</t>
-  </si>
-  <si>
-    <t>unpolarized</t>
-  </si>
-  <si>
     <t>C1, C2, C3, C10</t>
   </si>
   <si>
@@ -489,6 +477,18 @@
   </si>
   <si>
     <t>652-CRS0805FW1R00ELF</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>FTSH-105-01-F-D-K</t>
+  </si>
+  <si>
+    <t>SAM8909-ND</t>
+  </si>
+  <si>
+    <t>polarized</t>
   </si>
 </sst>
 </file>
@@ -948,8 +948,8 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1063,7 @@
         <v>11.95</v>
       </c>
       <c r="I3" s="6">
-        <f t="shared" ref="I3:I26" si="0">G3*H3</f>
+        <f t="shared" ref="I3:I25" si="0">G3*H3</f>
         <v>11.95</v>
       </c>
       <c r="J3" s="3"/>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>85</v>
@@ -1786,22 +1786,22 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>107</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E18" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G18" s="24">
         <v>1</v>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>116</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>61</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>67</v>
@@ -2041,22 +2041,22 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E23" s="30" t="s">
         <v>16</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G23" s="10">
         <v>1</v>
@@ -2092,22 +2092,22 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>68</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E24" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G24" s="10">
         <v>1</v>
@@ -2143,22 +2143,22 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E25" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G25" s="10">
         <v>1</v>
@@ -2171,7 +2171,7 @@
         <v>0.49</v>
       </c>
       <c r="J25" s="30" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K25" s="30" t="s">
         <v>23</v>
@@ -2200,29 +2200,29 @@
         <v>128</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="G26" s="10">
         <v>1</v>
       </c>
       <c r="H26" s="10">
-        <v>1.28</v>
+        <v>2.74</v>
       </c>
       <c r="I26" s="10">
         <f t="shared" ref="I26" si="1">G26*H26</f>
-        <v>1.28</v>
+        <v>2.74</v>
       </c>
       <c r="J26" s="30" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="K26" s="31" t="s">
         <v>23</v>
@@ -2254,7 +2254,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6">
         <f>SUM(I3:I26)</f>
-        <v>40.938000000000002</v>
+        <v>42.398000000000003</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
@@ -29464,6 +29464,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -29475,8 +29476,8 @@
   </sheetPr>
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:K8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29825,34 +29826,34 @@
         <v>128</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
       </c>
       <c r="H8" s="10">
-        <v>1.28</v>
+        <v>2.74</v>
       </c>
       <c r="I8" s="10">
         <f t="shared" si="0"/>
-        <v>1.28</v>
+        <v>2.74</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="K8" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="10"/>
+      <c r="L8" s="31"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>

</xml_diff>

<commit_message>
updated BoM with crystal
</commit_message>
<xml_diff>
--- a/New PCB, no jumpers/Bill of Materials.xlsx
+++ b/New PCB, no jumpers/Bill of Materials.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kpezeshki\Desktop\MuddPiV5\New PCB, no jumpers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kpezeshki\Desktop\MuddPIV5\New PCB, no jumpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850"/>
   </bookViews>
   <sheets>
     <sheet name="uMudd Mark V" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="161">
   <si>
     <t>https://www.segger.com/purchase/pricing/jlink-related/</t>
   </si>
@@ -419,9 +419,6 @@
     <t>2.2uF capacitor</t>
   </si>
   <si>
-    <t>C4, C6, C8, C11, C12, C13, C15</t>
-  </si>
-  <si>
     <t>C16</t>
   </si>
   <si>
@@ -489,6 +486,24 @@
   </si>
   <si>
     <t>polarized</t>
+  </si>
+  <si>
+    <t>C4, C6, C8, C11, C12, C13, C15, C17</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>40MHz oscillator</t>
+  </si>
+  <si>
+    <t>TXC Corporation</t>
+  </si>
+  <si>
+    <t>9B-40.000MAAJ-B</t>
+  </si>
+  <si>
+    <t>887-2030-ND</t>
   </si>
 </sst>
 </file>
@@ -948,13 +963,13 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="1" max="1" width="32.453125" customWidth="1"/>
     <col min="2" max="2" width="21.81640625" customWidth="1"/>
     <col min="4" max="4" width="23.7265625" customWidth="1"/>
   </cols>
@@ -1390,7 +1405,7 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>85</v>
@@ -1786,22 +1801,22 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>107</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E18" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G18" s="24">
         <v>1</v>
@@ -1837,7 +1852,7 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>116</v>
@@ -1888,7 +1903,7 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>61</v>
@@ -1906,14 +1921,14 @@
         <v>65</v>
       </c>
       <c r="G20" s="13">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H20" s="6">
         <v>0.1</v>
       </c>
       <c r="I20" s="6">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>24</v>
@@ -2047,16 +2062,16 @@
         <v>131</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E23" s="30" t="s">
         <v>16</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G23" s="10">
         <v>1</v>
@@ -2092,22 +2107,22 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>68</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E24" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G24" s="10">
         <v>1</v>
@@ -2143,22 +2158,22 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="30" t="s">
-        <v>136</v>
-      </c>
       <c r="C25" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E25" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G25" s="10">
         <v>1</v>
@@ -2171,7 +2186,7 @@
         <v>0.49</v>
       </c>
       <c r="J25" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K25" s="30" t="s">
         <v>23</v>
@@ -2200,16 +2215,16 @@
         <v>128</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E26" s="30" t="s">
         <v>16</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G26" s="10">
         <v>1</v>
@@ -2218,11 +2233,11 @@
         <v>2.74</v>
       </c>
       <c r="I26" s="10">
-        <f t="shared" ref="I26" si="1">G26*H26</f>
+        <f t="shared" ref="I26:I27" si="1">G26*H26</f>
         <v>2.74</v>
       </c>
       <c r="J26" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K26" s="31" t="s">
         <v>23</v>
@@ -2244,20 +2259,40 @@
       <c r="Z26" s="6"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6">
-        <f>SUM(I3:I26)</f>
-        <v>42.398000000000003</v>
+      <c r="A27" s="3" t="s">
+        <v>156</v>
       </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
+      <c r="B27" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="6">
+        <v>0.39</v>
+      </c>
+      <c r="I27" s="10">
+        <f t="shared" si="1"/>
+        <v>0.39</v>
+      </c>
+      <c r="J27" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="K27" s="30" t="s">
+        <v>23</v>
+      </c>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
@@ -2339,7 +2374,10 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+      <c r="I30" s="6">
+        <f>SUM(I3:I27)</f>
+        <v>43.088000000000001</v>
+      </c>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
@@ -29476,8 +29514,8 @@
   </sheetPr>
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29826,16 +29864,16 @@
         <v>128</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
@@ -29848,7 +29886,7 @@
         <v>2.74</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K8" s="31" t="s">
         <v>23</v>

</xml_diff>